<commit_message>
add Q&A problem about srpm compiled
</commit_message>
<xml_diff>
--- a/StarlingX_CentOS8.0_Kernel_Upgrade_Q&A List.xlsx
+++ b/StarlingX_CentOS8.0_Kernel_Upgrade_Q&A List.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>StarlingX CentOS8.0 Kernel upgrade Q&amp;A List</t>
   </si>
@@ -223,6 +223,66 @@
 Do you need to replace all of them with python3?</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t>Python-keystoneauth1 upgrade el8 compile dependency problem</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+Python-keystoneauth will depend on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t>python3-oslotest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> when compiling.
+Python3-oslotest will depend on python3-mox3 when compiling.
+Python3-mox3 will depend on python3-stestr when compiling.
+Python3-stestr will depend on python3-subunit2sql when compiling,
+Python3-subunit2sql will depend on python3-oslo-concurrency when compiling,
+However, python3-oslo-concurrency in turn depends on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+      </rPr>
+      <t>python3-oslotest</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.
+How should this work?</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -232,7 +292,7 @@
     <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-m\-d"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
@@ -291,6 +351,11 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="微软雅黑"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="微软雅黑"/>
     </font>
   </fonts>
@@ -1174,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1213,7 +1278,7 @@
       </c>
       <c r="K2" s="3">
         <f>COUNTA($C$6:$C$1998)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="2:11">
@@ -1222,7 +1287,7 @@
       </c>
       <c r="K3" s="3">
         <f>K2-COUNTIF($K$6:$K$1998,"OK")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="5.4" customHeight="1"/>
@@ -1400,11 +1465,21 @@
       <c r="B11" s="16">
         <v>6</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="C11" s="31">
+        <v>43787</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="H11" s="17"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>

</xml_diff>